<commit_message>
T4.1 lSS simple Some parts list stuff
</commit_message>
<xml_diff>
--- a/T41_LSS/T41SimpleLSSArduinoShieldV02 Parts List.xlsx
+++ b/T41_LSS/T41SimpleLSSArduinoShieldV02 Parts List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Teensy3.1-Breakout-Boards\T41_LSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B5F4F43-471C-4139-AD3B-F0E3016F53AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F5B442-88BB-4205-B8F8-F6925E83BF73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="2820" windowWidth="19500" windowHeight="17220" xr2:uid="{BCE9899B-7DDB-4A6A-967D-ED23F9D332DB}"/>
+    <workbookView xWindow="1905" yWindow="2970" windowWidth="20730" windowHeight="17220" xr2:uid="{BCE9899B-7DDB-4A6A-967D-ED23F9D332DB}"/>
   </bookViews>
   <sheets>
     <sheet name="T41SimpleLSSArduinoShieldV02" sheetId="2" r:id="rId1"/>
@@ -444,11 +444,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E7B7A0D-C4B9-4678-9421-6033A6A4A080}" name="T41SimpleLSSArduinoShieldV02" displayName="T41SimpleLSSArduinoShieldV02" ref="A1:G21" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:G21" xr:uid="{501BF650-08F4-43B8-9395-0B0C040A901D}"/>
   <tableColumns count="7">
-    <tableColumn id="7" xr3:uid="{8EED5790-0453-4C4B-A7DD-27982A587FD6}" uniqueName="7" name="Part Numbers (Digikey)" queryTableFieldId="7" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{B967E0CC-8631-457B-BBC1-B63C628238C0}" uniqueName="1" name="RefDes" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{52D072DD-44E9-440D-9676-69E18D7F3AB5}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{E235ECF8-9A9F-4E41-A435-EA26D0244DF0}" uniqueName="3" name="Pattern" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{E5F34D7A-D1E8-4C05-B7DD-087B862F17E3}" uniqueName="4" name="Value" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{8EED5790-0453-4C4B-A7DD-27982A587FD6}" uniqueName="7" name="Part Numbers (Digikey)" queryTableFieldId="7" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{B967E0CC-8631-457B-BBC1-B63C628238C0}" uniqueName="1" name="RefDes" queryTableFieldId="1" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{52D072DD-44E9-440D-9676-69E18D7F3AB5}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{E235ECF8-9A9F-4E41-A435-EA26D0244DF0}" uniqueName="3" name="Pattern" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{E5F34D7A-D1E8-4C05-B7DD-087B862F17E3}" uniqueName="4" name="Value" queryTableFieldId="4" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{CAF4E0E2-A139-46B7-B91B-1FD4A31D6AA1}" uniqueName="5" name="Number of Pins" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{69568E6A-3ED2-48E5-A806-AB8B2F22DBE5}" uniqueName="6" name="Quantity" queryTableFieldId="6"/>
   </tableColumns>
@@ -756,7 +756,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update T41SimpleLSSArduinoShieldV02 Parts List.xlsx
Wrong Qwiic part for the pattern used on board
</commit_message>
<xml_diff>
--- a/T41_LSS/T41SimpleLSSArduinoShieldV02 Parts List.xlsx
+++ b/T41_LSS/T41SimpleLSSArduinoShieldV02 Parts List.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Teensy3.1-Breakout-Boards\T41_LSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F5B442-88BB-4205-B8F8-F6925E83BF73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C473D871-C2A2-4B3B-AE50-1F74BF4E6623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="2970" windowWidth="20730" windowHeight="17220" xr2:uid="{BCE9899B-7DDB-4A6A-967D-ED23F9D332DB}"/>
+    <workbookView xWindow="6705" yWindow="1935" windowWidth="30210" windowHeight="18585" xr2:uid="{BCE9899B-7DDB-4A6A-967D-ED23F9D332DB}"/>
   </bookViews>
   <sheets>
     <sheet name="T41SimpleLSSArduinoShieldV02" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">T41SimpleLSSArduinoShieldV02!$B$1:$G$21</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">T41SimpleLSSArduinoShieldV02!$B$1:$G$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
   <si>
     <t>RefDes</t>
   </si>
@@ -291,13 +291,19 @@
   </si>
   <si>
     <t>811-2692-ND</t>
+  </si>
+  <si>
+    <t>Sparkfun #14417</t>
+  </si>
+  <si>
+    <t>Qwiic JST Connector Horizontal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +321,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -376,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -391,6 +405,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,8 +457,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E7B7A0D-C4B9-4678-9421-6033A6A4A080}" name="T41SimpleLSSArduinoShieldV02" displayName="T41SimpleLSSArduinoShieldV02" ref="A1:G21" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G21" xr:uid="{501BF650-08F4-43B8-9395-0B0C040A901D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E7B7A0D-C4B9-4678-9421-6033A6A4A080}" name="T41SimpleLSSArduinoShieldV02" displayName="T41SimpleLSSArduinoShieldV02" ref="A1:G22" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G22" xr:uid="{501BF650-08F4-43B8-9395-0B0C040A901D}"/>
   <tableColumns count="7">
     <tableColumn id="7" xr3:uid="{8EED5790-0453-4C4B-A7DD-27982A587FD6}" uniqueName="7" name="Part Numbers (Digikey)" queryTableFieldId="7" dataDxfId="4"/>
     <tableColumn id="1" xr3:uid="{B967E0CC-8631-457B-BBC1-B63C628238C0}" uniqueName="1" name="RefDes" queryTableFieldId="1" dataDxfId="3"/>
@@ -753,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B263D98F-0E35-48AB-9709-9E91FF435122}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1000,84 +1016,84 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
         <v>4</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>80</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>9</v>
@@ -1090,80 +1106,80 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>76</v>
+      <c r="A15" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>77</v>
+      <c r="A16" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="F16">
         <v>3</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>50</v>
@@ -1172,7 +1188,7 @@
         <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F18">
         <v>2</v>
@@ -1182,17 +1198,17 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>79</v>
+      <c r="A19" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>53</v>
@@ -1201,52 +1217,75 @@
         <v>2</v>
       </c>
       <c r="G19">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>74</v>
+      <c r="A20" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>2</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>57</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>1</v>
       </c>
     </row>

</xml_diff>